<commit_message>
Update on Nicole's file.
</commit_message>
<xml_diff>
--- a/SolrScripts/results-gc/set-verifying/verifying-set-nicole.xlsx
+++ b/SolrScripts/results-gc/set-verifying/verifying-set-nicole.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\febert\Documents\workspaces\solr\SolrScripts\results-gc\set-verifying\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="15456"/>
   </bookViews>
   <sheets>
     <sheet name="hedges" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="920">
   <si>
     <t>id</t>
   </si>
@@ -3521,6 +3518,9 @@
   </si>
   <si>
     <t>Request?</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -3643,13 +3643,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale visitato" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -3970,19 +3970,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B425" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D431" sqref="D431"/>
+    <sheetView tabSelected="1" topLeftCell="B415" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C422" sqref="C422"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="79" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="64.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>871</v>
       </c>
@@ -3990,7 +3990,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>802</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>806</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>809</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>812</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>816</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>818</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>821</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>824</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>826</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>829</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>831</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>834</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>837</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>840</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>843</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>846</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>849</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>852</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>854</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>856</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="132" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>859</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>862</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>865</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>867</v>
       </c>
@@ -4340,7 +4340,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>869</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="169" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -4584,7 +4584,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:4" ht="132" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="195" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:4" ht="198" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -4810,7 +4810,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>84</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>92</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>96</v>
       </c>
@@ -4912,7 +4912,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="247" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:4" ht="250.8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>100</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>104</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>106</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>108</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="78" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>110</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>112</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>114</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>116</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>118</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="104" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>120</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>124</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>126</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>128</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>130</v>
       </c>
@@ -5099,7 +5099,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>132</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="104" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>134</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>136</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>138</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>140</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>142</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>144</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>146</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>152</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>154</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>156</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>158</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>160</v>
       </c>
@@ -5273,7 +5273,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>162</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>164</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>168</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>170</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>172</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>174</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>176</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>178</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>180</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>182</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>184</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>186</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>188</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>190</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>192</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>194</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>196</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>198</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>200</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>202</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>204</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>206</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>210</v>
       </c>
@@ -5560,7 +5560,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>212</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="143" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>214</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>216</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>218</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>220</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>222</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>224</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="182" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:4" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>226</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>228</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>230</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>232</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>234</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>236</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>238</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>240</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>242</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>244</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>246</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>248</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>250</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>252</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>254</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>256</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>258</v>
       </c>
@@ -5833,7 +5833,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>260</v>
       </c>
@@ -5847,7 +5847,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>262</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>264</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>266</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>268</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>270</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>272</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>274</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>276</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>278</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>280</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>282</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>284</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>286</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>288</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>290</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>292</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>294</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>296</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>298</v>
       </c>
@@ -6062,7 +6062,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>300</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>302</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>304</v>
       </c>
@@ -6095,7 +6095,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>306</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>308</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>310</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>312</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>314</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>316</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>318</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>320</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>322</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>324</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>326</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>328</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>330</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>332</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>334</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>336</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>338</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>340</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>342</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>344</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>346</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="182" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:4" ht="198" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>348</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>350</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>352</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="129" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:4" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>354</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>356</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>358</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>360</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>362</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>364</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>366</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>368</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>370</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>372</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>374</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>376</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>378</v>
       </c>
@@ -6520,7 +6520,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>380</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>382</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>384</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>386</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>388</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>390</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="225" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>392</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>394</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>396</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>398</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>400</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>402</v>
       </c>
@@ -6652,7 +6652,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="130" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>404</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>406</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="233" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>408</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>410</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="235" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>412</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="236" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>414</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>416</v>
       </c>
@@ -6729,7 +6729,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>418</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="239" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>420</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="240" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>422</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="241" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>424</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="242" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>426</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="243" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>428</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>430</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="245" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>432</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="246" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>434</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="247" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>436</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="248" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>438</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="249" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>440</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="250" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>442</v>
       </c>
@@ -6872,7 +6872,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>444</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="252" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>446</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="253" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>448</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="254" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>450</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="255" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>452</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="256" spans="1:3" ht="78" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>454</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="257" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>456</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="258" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>458</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="259" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>460</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="260" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>462</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="261" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>464</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="262" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>466</v>
       </c>
@@ -7007,7 +7007,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="263" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>468</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="264" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>470</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="265" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>472</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="266" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>474</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="267" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>476</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="268" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>478</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="269" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>480</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>482</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="271" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>484</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="272" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>486</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="273" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>488</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="274" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>490</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="275" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>492</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="276" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>494</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="277" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>496</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>498</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>500</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="280" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>502</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="281" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>504</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="282" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>506</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="283" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>508</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>510</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>512</v>
       </c>
@@ -7275,7 +7275,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>514</v>
       </c>
@@ -7286,7 +7286,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>516</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="288" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>518</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>520</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="290" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>522</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>524</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>526</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="293" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>528</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="294" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>530</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="295" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>532</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="296" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>534</v>
       </c>
@@ -7396,7 +7396,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="297" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>536</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="298" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>538</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>540</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="300" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>542</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>544</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>546</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="303" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>548</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="304" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>550</v>
       </c>
@@ -7487,7 +7487,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>552</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>554</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>556</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>558</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>560</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>562</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>564</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>566</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>568</v>
       </c>
@@ -7595,7 +7595,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>570</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>572</v>
       </c>
@@ -7620,7 +7620,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>574</v>
       </c>
@@ -7631,7 +7631,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>576</v>
       </c>
@@ -7642,7 +7642,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>578</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>580</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>582</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="321" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>584</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="322" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>586</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="323" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>588</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="324" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>590</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>592</v>
       </c>
@@ -7736,7 +7736,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="326" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>594</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="327" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>596</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="328" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>598</v>
       </c>
@@ -7769,7 +7769,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="329" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>600</v>
       </c>
@@ -7783,7 +7783,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="330" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>602</v>
       </c>
@@ -7797,7 +7797,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="331" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>604</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>606</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="333" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>608</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="334" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>610</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="335" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>612</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="336" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>614</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="337" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>616</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="338" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>618</v>
       </c>
@@ -7888,7 +7888,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="339" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>620</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="340" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>622</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="341" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>624</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="342" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>626</v>
       </c>
@@ -7935,7 +7935,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="343" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>628</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="344" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>630</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="345" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>632</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>634</v>
       </c>
@@ -7985,7 +7985,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="347" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>636</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="348" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>638</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="349" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>640</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="350" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>642</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="351" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>644</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="352" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>646</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="353" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>648</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="354" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>650</v>
       </c>
@@ -8073,7 +8073,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="355" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>652</v>
       </c>
@@ -8084,7 +8084,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="356" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>654</v>
       </c>
@@ -8095,7 +8095,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="357" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>656</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="358" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>658</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="359" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>660</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="360" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>662</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="361" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="361" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>664</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="362" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>666</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="363" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>668</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="364" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="364" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>670</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="365" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="365" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>672</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="366" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="366" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>674</v>
       </c>
@@ -8205,7 +8205,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="367" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="367" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>676</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="368" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="368" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>678</v>
       </c>
@@ -8230,7 +8230,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="369" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="369" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>680</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="370" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="370" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>682</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="371" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="371" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>684</v>
       </c>
@@ -8266,7 +8266,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="372" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>686</v>
       </c>
@@ -8277,7 +8277,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="373" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="373" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>688</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="374" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="374" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>690</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="375" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="375" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>692</v>
       </c>
@@ -8313,7 +8313,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="376" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="376" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>694</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="377" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="377" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>696</v>
       </c>
@@ -8335,7 +8335,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="378" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="378" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>698</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="379" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="379" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>700</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="380" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="380" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>702</v>
       </c>
@@ -8368,7 +8368,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="381" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="381" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>703</v>
       </c>
@@ -8379,7 +8379,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="382" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="382" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>705</v>
       </c>
@@ -8390,7 +8390,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="383" spans="1:4" ht="26" x14ac:dyDescent="0.15">
+    <row r="383" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>707</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="384" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="384" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>709</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="385" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="385" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>711</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="386" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="386" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>713</v>
       </c>
@@ -8434,7 +8434,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="387" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="387" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>715</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="388" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="388" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>717</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="389" spans="1:3" ht="52" x14ac:dyDescent="0.15">
+    <row r="389" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>719</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="390" spans="1:3" ht="104" x14ac:dyDescent="0.15">
+    <row r="390" spans="1:3" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>721</v>
       </c>
@@ -8478,7 +8478,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="391" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="391" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>723</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="392" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="392" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>725</v>
       </c>
@@ -8500,7 +8500,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="393" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="393" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>727</v>
       </c>
@@ -8511,7 +8511,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="394" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="394" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>729</v>
       </c>
@@ -8522,7 +8522,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="395" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="395" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>731</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="396" spans="1:3" ht="91" x14ac:dyDescent="0.15">
+    <row r="396" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>732</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="397" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="397" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>734</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="398" spans="1:3" ht="65" x14ac:dyDescent="0.15">
+    <row r="398" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>736</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="399" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="399" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>738</v>
       </c>
@@ -8577,7 +8577,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="400" spans="1:3" ht="39" x14ac:dyDescent="0.15">
+    <row r="400" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>740</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="401" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="401" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>742</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="402" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>744</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="403" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="403" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>746</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="404" spans="1:4" ht="169" x14ac:dyDescent="0.15">
+    <row r="404" spans="1:4" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>748</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="405" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="405" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>750</v>
       </c>
@@ -8643,7 +8643,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="406" spans="1:4" ht="156" x14ac:dyDescent="0.15">
+    <row r="406" spans="1:4" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>752</v>
       </c>
@@ -8654,7 +8654,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="407" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>754</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="408" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>756</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="409" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="409" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>758</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="410" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="410" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>760</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="411" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="411" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>762</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="412" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="412" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>764</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="413" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="413" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>766</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="414" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="414" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>768</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="415" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="415" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>770</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="416" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="416" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>772</v>
       </c>
@@ -8776,7 +8776,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="417" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="417" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>774</v>
       </c>
@@ -8787,7 +8787,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="418" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="418" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>776</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="419" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="419" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>778</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="420" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="420" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>780</v>
       </c>
@@ -8820,16 +8820,18 @@
         <v>803</v>
       </c>
     </row>
-    <row r="421" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="421" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>782</v>
       </c>
       <c r="B421" s="4" t="s">
         <v>783</v>
       </c>
-      <c r="C421" s="2"/>
-    </row>
-    <row r="422" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+      <c r="C421" s="2" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>784</v>
       </c>
@@ -8840,7 +8842,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="423" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="423" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>786</v>
       </c>
@@ -8851,7 +8853,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="424" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="424" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>788</v>
       </c>
@@ -8862,7 +8864,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="425" spans="1:4" ht="117" x14ac:dyDescent="0.15">
+    <row r="425" spans="1:4" ht="132" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>790</v>
       </c>
@@ -8873,7 +8875,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="426" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="426" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>792</v>
       </c>
@@ -8884,7 +8886,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="427" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="427" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>794</v>
       </c>
@@ -8898,7 +8900,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="428" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="428" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>796</v>
       </c>
@@ -8909,7 +8911,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="429" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="429" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>798</v>
       </c>
@@ -8920,7 +8922,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="430" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="430" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>800</v>
       </c>
@@ -8959,14 +8961,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="85" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.5" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>871</v>
       </c>
@@ -8974,7 +8976,7 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -8988,7 +8990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="104" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>802</v>
       </c>
@@ -9002,7 +9004,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>806</v>
       </c>
@@ -9016,7 +9018,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>809</v>
       </c>
@@ -9030,7 +9032,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>812</v>
       </c>
@@ -9044,7 +9046,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>816</v>
       </c>
@@ -9058,7 +9060,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>818</v>
       </c>
@@ -9072,7 +9074,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>821</v>
       </c>
@@ -9086,7 +9088,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="91" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>824</v>
       </c>
@@ -9100,7 +9102,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>826</v>
       </c>
@@ -9114,7 +9116,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>829</v>
       </c>
@@ -9128,7 +9130,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>831</v>
       </c>
@@ -9142,7 +9144,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>834</v>
       </c>
@@ -9156,7 +9158,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>837</v>
       </c>
@@ -9170,7 +9172,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>840</v>
       </c>
@@ -9184,7 +9186,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>843</v>
       </c>
@@ -9198,7 +9200,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>846</v>
       </c>
@@ -9212,7 +9214,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>849</v>
       </c>
@@ -9226,7 +9228,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>852</v>
       </c>
@@ -9240,7 +9242,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>854</v>
       </c>
@@ -9254,7 +9256,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>856</v>
       </c>
@@ -9268,7 +9270,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="130" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="132" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>859</v>
       </c>
@@ -9282,7 +9284,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>862</v>
       </c>
@@ -9296,7 +9298,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>865</v>
       </c>
@@ -9310,7 +9312,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="78" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>867</v>
       </c>
@@ -9324,7 +9326,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="39" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>869</v>
       </c>

</xml_diff>